<commit_message>
altered formatting on dCIN5 log sheet
Changed the headers from center alignment to right alignment. Although it included the dcin5 and wt strains already on the optimization_parameters sheet, I added the other strain's information as well.
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/15-genes_20-edges_NW-dCIN5-fam_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/15-genes_20-edges_NW-dCIN5-fam_Sigmoid_estimation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwilli31\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="25365" windowHeight="13725" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" tabRatio="500" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="3" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="86">
   <si>
     <t>ACE2</t>
   </si>
@@ -269,10 +274,19 @@
     <t>wt</t>
   </si>
   <si>
-    <t>cin5</t>
-  </si>
-  <si>
     <t>rows genes affected/cols genes controlling</t>
+  </si>
+  <si>
+    <t>dcin5</t>
+  </si>
+  <si>
+    <t>dgln3</t>
+  </si>
+  <si>
+    <t>dhap4</t>
+  </si>
+  <si>
+    <t>dzap1</t>
   </si>
 </sst>
 </file>
@@ -368,7 +382,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -395,6 +409,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,6 +425,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -736,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -879,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -911,7 +932,7 @@
       <c r="A3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1017,7 +1038,16 @@
         <v>80</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1074,7 +1104,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1248,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2123,7 +2153,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2139,41 +2169,41 @@
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11">
+      <c r="B1" s="18">
         <v>15</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="18">
         <v>15</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="18">
         <v>15</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="18">
         <v>15</v>
       </c>
-      <c r="F1" s="11">
-        <v>30</v>
-      </c>
-      <c r="G1" s="11">
-        <v>30</v>
-      </c>
-      <c r="H1" s="11">
-        <v>30</v>
-      </c>
-      <c r="I1" s="11">
-        <v>30</v>
-      </c>
-      <c r="J1" s="11">
-        <v>60</v>
-      </c>
-      <c r="K1" s="11">
-        <v>60</v>
-      </c>
-      <c r="L1" s="11">
-        <v>60</v>
-      </c>
-      <c r="M1" s="11">
-        <v>60</v>
+      <c r="F1" s="18">
+        <v>15</v>
+      </c>
+      <c r="G1" s="18">
+        <v>15</v>
+      </c>
+      <c r="H1" s="18">
+        <v>15</v>
+      </c>
+      <c r="I1" s="18">
+        <v>15</v>
+      </c>
+      <c r="J1" s="18">
+        <v>15</v>
+      </c>
+      <c r="K1" s="18">
+        <v>15</v>
+      </c>
+      <c r="L1" s="18">
+        <v>15</v>
+      </c>
+      <c r="M1" s="18">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -2815,7 +2845,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3489,7 +3519,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4160,7 +4190,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4843,7 +4873,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4853,7 +4883,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -5676,7 +5706,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
altered dCIN5 log expression sheet
Changed the headings for the dCIN5 expression data because they were all 15s with no 30s or 60s
</commit_message>
<xml_diff>
--- a/data/GRNmap_input_workbooks/15-genes_20-edges_NW-dCIN5-fam_Sigmoid_estimation.xlsx
+++ b/data/GRNmap_input_workbooks/15-genes_20-edges_NW-dCIN5-fam_Sigmoid_estimation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwilli31\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwilli31\Documents\GRNmap\matlab_dCIN5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" tabRatio="500" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="optimization_parameters" sheetId="10" r:id="rId10"/>
     <sheet name="threshold_b" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -758,7 +758,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>-0.22359999999999999</v>
+        <v>0.22359999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>-0.20100000000000001</v>
+        <v>0.20100000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +792,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>-0.19259999999999999</v>
+        <v>0.19259999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>-0.32240000000000002</v>
+        <v>0.32240000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>-0.27179999999999999</v>
+        <v>0.27179999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>-0.19800000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>-0.4078</v>
+        <v>0.4078</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>-0.21659999999999999</v>
+        <v>0.21659999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>-0.19800000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>-0.69320000000000004</v>
+        <v>0.69320000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>-0.14000000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>-0.32240000000000002</v>
+        <v>0.32240000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>-0.17319999999999999</v>
+        <v>0.17319999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>-0.72960000000000003</v>
+        <v>0.72960000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>-0.1042</v>
+        <v>0.1042</v>
       </c>
     </row>
   </sheetData>
@@ -900,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -1248,7 +1248,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="15">
-        <v>-0.1118</v>
+        <v>0.1118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="15">
-        <v>-0.10050000000000001</v>
+        <v>0.10050000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="15">
-        <v>-9.6299999999999997E-2</v>
+        <v>9.6299999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1293,7 +1293,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="15">
-        <v>-0.16120000000000001</v>
+        <v>0.16120000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1301,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="15">
-        <v>-0.13589999999999999</v>
+        <v>0.13589999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="16">
-        <v>-9.9000000000000005E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="15">
-        <v>-0.2039</v>
+        <v>0.2039</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1325,7 +1325,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="15">
-        <v>-0.10829999999999999</v>
+        <v>0.10829999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1333,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="16">
-        <v>-9.9000000000000005E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1341,7 +1341,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="15">
-        <v>-0.34660000000000002</v>
+        <v>0.34660000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1349,7 +1349,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="17">
-        <v>-7.0000000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1357,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="15">
-        <v>-0.16120000000000001</v>
+        <v>0.16120000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1365,7 +1365,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="15">
-        <v>-8.6599999999999996E-2</v>
+        <v>8.6599999999999996E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1373,7 +1373,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="15">
-        <v>-0.36480000000000001</v>
+        <v>0.36480000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1381,7 +1381,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="15">
-        <v>-5.21E-2</v>
+        <v>5.21E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1395,7 +1395,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2153,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2182,28 +2182,28 @@
         <v>15</v>
       </c>
       <c r="F1" s="18">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G1" s="18">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H1" s="18">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I1" s="18">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J1" s="18">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K1" s="18">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="L1" s="18">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="M1" s="18">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -2845,7 +2845,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3518,8 +3518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>